<commit_message>
changed resistor values in schematic
</commit_message>
<xml_diff>
--- a/src/schematics/Mayo_Phantom/Resistor Phantom/Resistor_Phantom_BOM.xlsx
+++ b/src/schematics/Mayo_Phantom/Resistor Phantom/Resistor_Phantom_BOM.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="206">
   <si>
     <t>Part</t>
   </si>
@@ -581,9 +581,6 @@
     <t>R163</t>
   </si>
   <si>
-    <t>300k</t>
-  </si>
-  <si>
     <t>R164</t>
   </si>
   <si>
@@ -596,15 +593,9 @@
     <t>R171</t>
   </si>
   <si>
-    <t>9k</t>
-  </si>
-  <si>
     <t>R172</t>
   </si>
   <si>
-    <t>30k</t>
-  </si>
-  <si>
     <t>R173</t>
   </si>
   <si>
@@ -638,27 +629,6 @@
     <t>MC00625W04021510R</t>
   </si>
   <si>
-    <t>MC00625W0402130K</t>
-  </si>
-  <si>
-    <t>MC00625W04021300K</t>
-  </si>
-  <si>
-    <t>75k</t>
-  </si>
-  <si>
-    <t>24k</t>
-  </si>
-  <si>
-    <t>MC00625W0402175K</t>
-  </si>
-  <si>
-    <t>MC00625W0402124K</t>
-  </si>
-  <si>
-    <t>MC00625W040219K1</t>
-  </si>
-  <si>
     <t>AQY221R2S</t>
   </si>
   <si>
@@ -675,13 +645,34 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>0402-100R</t>
+  </si>
+  <si>
+    <t>0402-510R</t>
+  </si>
+  <si>
+    <t>0402-200R</t>
+  </si>
+  <si>
+    <t>0402-2K</t>
+  </si>
+  <si>
+    <t>0402-10K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -694,6 +685,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -716,12 +713,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,19 +1041,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="H188" sqref="H188"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="F165" sqref="F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1046,7 +1079,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1054,19 +1087,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="G2">
         <v>1653770</v>
@@ -1077,19 +1110,19 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D3" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="G3">
         <v>1653770</v>
@@ -1100,19 +1133,19 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D4" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="G4">
         <v>1653770</v>
@@ -1135,13 +1168,13 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G5" s="1">
         <v>1358043</v>
       </c>
       <c r="H5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1161,13 +1194,13 @@
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G6" s="1">
         <v>1358043</v>
       </c>
       <c r="H6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1187,13 +1220,13 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G7" s="1">
         <v>1358043</v>
       </c>
       <c r="H7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1213,13 +1246,13 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G8" s="1">
         <v>1358043</v>
       </c>
       <c r="H8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1239,13 +1272,13 @@
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G9" s="1">
         <v>1358043</v>
       </c>
       <c r="H9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1265,13 +1298,13 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G10" s="1">
         <v>1358043</v>
       </c>
       <c r="H10" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1291,13 +1324,13 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G11" s="1">
         <v>1358043</v>
       </c>
       <c r="H11" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1317,13 +1350,13 @@
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G12" s="1">
         <v>1358043</v>
       </c>
       <c r="H12" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1343,13 +1376,13 @@
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G13" s="1">
         <v>1358043</v>
       </c>
       <c r="H13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1369,13 +1402,13 @@
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G14" s="1">
         <v>1358043</v>
       </c>
       <c r="H14" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1395,13 +1428,13 @@
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G15" s="1">
         <v>1358043</v>
       </c>
       <c r="H15" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1421,13 +1454,13 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G16" s="1">
         <v>1358043</v>
       </c>
       <c r="H16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1447,13 +1480,13 @@
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G17" s="1">
         <v>1358043</v>
       </c>
       <c r="H17" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1473,13 +1506,13 @@
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G18" s="1">
         <v>1358043</v>
       </c>
       <c r="H18" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1499,13 +1532,13 @@
         <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G19" s="1">
         <v>1358043</v>
       </c>
       <c r="H19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1525,13 +1558,13 @@
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G20" s="1">
         <v>1358043</v>
       </c>
       <c r="H20" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1551,13 +1584,13 @@
         <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G21" s="1">
         <v>1358043</v>
       </c>
       <c r="H21" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1577,13 +1610,13 @@
         <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G22" s="1">
         <v>1358043</v>
       </c>
       <c r="H22" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1603,13 +1636,13 @@
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G23" s="1">
         <v>1358043</v>
       </c>
       <c r="H23" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1629,13 +1662,13 @@
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G24" s="1">
         <v>1358043</v>
       </c>
       <c r="H24" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1655,13 +1688,13 @@
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G25" s="1">
         <v>1358043</v>
       </c>
       <c r="H25" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1681,13 +1714,13 @@
         <v>15</v>
       </c>
       <c r="F26" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G26" s="1">
         <v>1358043</v>
       </c>
       <c r="H26" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1707,13 +1740,13 @@
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G27" s="1">
         <v>1358043</v>
       </c>
       <c r="H27" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1733,13 +1766,13 @@
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G28" s="1">
         <v>1358043</v>
       </c>
       <c r="H28" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1759,13 +1792,13 @@
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G29" s="1">
         <v>1358043</v>
       </c>
       <c r="H29" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1785,13 +1818,13 @@
         <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G30" s="1">
         <v>1358043</v>
       </c>
       <c r="H30" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1811,13 +1844,13 @@
         <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G31" s="1">
         <v>1358043</v>
       </c>
       <c r="H31" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1837,13 +1870,13 @@
         <v>15</v>
       </c>
       <c r="F32" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G32" s="1">
         <v>1358043</v>
       </c>
       <c r="H32" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1863,13 +1896,13 @@
         <v>15</v>
       </c>
       <c r="F33" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G33" s="1">
         <v>1358043</v>
       </c>
       <c r="H33" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1889,13 +1922,13 @@
         <v>15</v>
       </c>
       <c r="F34" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G34" s="1">
         <v>1358043</v>
       </c>
       <c r="H34" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1915,13 +1948,13 @@
         <v>15</v>
       </c>
       <c r="F35" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G35" s="1">
         <v>1358043</v>
       </c>
       <c r="H35" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1941,13 +1974,13 @@
         <v>15</v>
       </c>
       <c r="F36" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G36" s="1">
         <v>1358043</v>
       </c>
       <c r="H36" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1967,13 +2000,13 @@
         <v>15</v>
       </c>
       <c r="F37" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G37" s="1">
         <v>1358043</v>
       </c>
       <c r="H37" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1993,13 +2026,13 @@
         <v>15</v>
       </c>
       <c r="F38" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G38" s="1">
         <v>1358043</v>
       </c>
       <c r="H38" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2019,13 +2052,13 @@
         <v>15</v>
       </c>
       <c r="F39" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G39" s="1">
         <v>1358043</v>
       </c>
       <c r="H39" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2045,13 +2078,13 @@
         <v>15</v>
       </c>
       <c r="F40" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G40" s="1">
         <v>1358043</v>
       </c>
       <c r="H40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2071,13 +2104,13 @@
         <v>15</v>
       </c>
       <c r="F41" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G41" s="1">
         <v>1358043</v>
       </c>
       <c r="H41" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2097,13 +2130,13 @@
         <v>15</v>
       </c>
       <c r="F42" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G42" s="1">
         <v>1358043</v>
       </c>
       <c r="H42" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2123,13 +2156,13 @@
         <v>15</v>
       </c>
       <c r="F43" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G43" s="1">
         <v>1358043</v>
       </c>
       <c r="H43" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2149,13 +2182,13 @@
         <v>15</v>
       </c>
       <c r="F44" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G44" s="1">
         <v>1358043</v>
       </c>
       <c r="H44" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2175,13 +2208,13 @@
         <v>15</v>
       </c>
       <c r="F45" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G45" s="1">
         <v>1358043</v>
       </c>
       <c r="H45" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2201,13 +2234,13 @@
         <v>15</v>
       </c>
       <c r="F46" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G46" s="1">
         <v>1358043</v>
       </c>
       <c r="H46" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2227,13 +2260,13 @@
         <v>15</v>
       </c>
       <c r="F47" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G47" s="1">
         <v>1358043</v>
       </c>
       <c r="H47" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2253,13 +2286,13 @@
         <v>15</v>
       </c>
       <c r="F48" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G48" s="1">
         <v>1358043</v>
       </c>
       <c r="H48" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2279,13 +2312,13 @@
         <v>15</v>
       </c>
       <c r="F49" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G49" s="1">
         <v>1358043</v>
       </c>
       <c r="H49" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2305,13 +2338,13 @@
         <v>15</v>
       </c>
       <c r="F50" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G50" s="1">
         <v>1358043</v>
       </c>
       <c r="H50" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2331,13 +2364,13 @@
         <v>15</v>
       </c>
       <c r="F51" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G51" s="1">
         <v>1358043</v>
       </c>
       <c r="H51" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2357,13 +2390,13 @@
         <v>15</v>
       </c>
       <c r="F52" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G52" s="1">
         <v>1358043</v>
       </c>
       <c r="H52" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2383,13 +2416,13 @@
         <v>15</v>
       </c>
       <c r="F53" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G53" s="1">
         <v>1358043</v>
       </c>
       <c r="H53" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2409,13 +2442,13 @@
         <v>15</v>
       </c>
       <c r="F54" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G54" s="1">
         <v>1358043</v>
       </c>
       <c r="H54" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2435,13 +2468,13 @@
         <v>15</v>
       </c>
       <c r="F55" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G55" s="1">
         <v>1358043</v>
       </c>
       <c r="H55" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2461,13 +2494,13 @@
         <v>15</v>
       </c>
       <c r="F56" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G56" s="1">
         <v>1358043</v>
       </c>
       <c r="H56" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2487,13 +2520,13 @@
         <v>15</v>
       </c>
       <c r="F57" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G57" s="1">
         <v>1358043</v>
       </c>
       <c r="H57" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2513,13 +2546,13 @@
         <v>15</v>
       </c>
       <c r="F58" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G58" s="1">
         <v>1358043</v>
       </c>
       <c r="H58" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2539,13 +2572,13 @@
         <v>15</v>
       </c>
       <c r="F59" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G59" s="1">
         <v>1358043</v>
       </c>
       <c r="H59" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2565,13 +2598,13 @@
         <v>15</v>
       </c>
       <c r="F60" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G60" s="1">
         <v>1358043</v>
       </c>
       <c r="H60" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2591,13 +2624,13 @@
         <v>15</v>
       </c>
       <c r="F61" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G61" s="1">
         <v>1358043</v>
       </c>
       <c r="H61" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2617,13 +2650,13 @@
         <v>15</v>
       </c>
       <c r="F62" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G62" s="1">
         <v>1358043</v>
       </c>
       <c r="H62" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2643,13 +2676,13 @@
         <v>15</v>
       </c>
       <c r="F63" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G63" s="1">
         <v>1358043</v>
       </c>
       <c r="H63" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2669,13 +2702,13 @@
         <v>15</v>
       </c>
       <c r="F64" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G64" s="1">
         <v>1358043</v>
       </c>
       <c r="H64" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2695,13 +2728,13 @@
         <v>15</v>
       </c>
       <c r="F65" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G65" s="1">
         <v>1358043</v>
       </c>
       <c r="H65" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2721,13 +2754,13 @@
         <v>15</v>
       </c>
       <c r="F66" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G66" s="1">
         <v>1358043</v>
       </c>
       <c r="H66" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2747,13 +2780,13 @@
         <v>15</v>
       </c>
       <c r="F67" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G67" s="1">
         <v>1358043</v>
       </c>
       <c r="H67" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2773,13 +2806,13 @@
         <v>15</v>
       </c>
       <c r="F68" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G68" s="1">
         <v>1358043</v>
       </c>
       <c r="H68" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2799,13 +2832,13 @@
         <v>15</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G69" s="1">
         <v>2130389</v>
       </c>
       <c r="H69" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2825,13 +2858,13 @@
         <v>15</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G70" s="1">
         <v>2130389</v>
       </c>
       <c r="H70" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2851,13 +2884,13 @@
         <v>15</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G71" s="1">
         <v>2130389</v>
       </c>
       <c r="H71" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2877,13 +2910,13 @@
         <v>15</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G72" s="1">
         <v>2130389</v>
       </c>
       <c r="H72" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2903,13 +2936,13 @@
         <v>15</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G73" s="1">
         <v>2130389</v>
       </c>
       <c r="H73" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2929,13 +2962,13 @@
         <v>15</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G74" s="1">
         <v>2130389</v>
       </c>
       <c r="H74" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2955,13 +2988,13 @@
         <v>15</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G75" s="1">
         <v>2130389</v>
       </c>
       <c r="H75" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2981,13 +3014,13 @@
         <v>15</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G76" s="1">
         <v>2130389</v>
       </c>
       <c r="H76" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3007,13 +3040,13 @@
         <v>15</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G77" s="1">
         <v>2130389</v>
       </c>
       <c r="H77" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3033,13 +3066,13 @@
         <v>15</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G78" s="1">
         <v>2130389</v>
       </c>
       <c r="H78" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3059,13 +3092,13 @@
         <v>15</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G79" s="1">
         <v>2130389</v>
       </c>
       <c r="H79" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3085,13 +3118,13 @@
         <v>15</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G80" s="1">
         <v>2130389</v>
       </c>
       <c r="H80" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3111,13 +3144,13 @@
         <v>15</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G81" s="1">
         <v>2130389</v>
       </c>
       <c r="H81" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3137,13 +3170,13 @@
         <v>15</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G82" s="1">
         <v>2130389</v>
       </c>
       <c r="H82" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3163,13 +3196,13 @@
         <v>15</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G83" s="1">
         <v>2130389</v>
       </c>
       <c r="H83" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3189,13 +3222,13 @@
         <v>15</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G84" s="1">
         <v>2130389</v>
       </c>
       <c r="H84" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3215,13 +3248,13 @@
         <v>15</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G85" s="1">
         <v>2130389</v>
       </c>
       <c r="H85" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3241,13 +3274,13 @@
         <v>15</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G86" s="1">
         <v>2130389</v>
       </c>
       <c r="H86" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3267,13 +3300,13 @@
         <v>15</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G87" s="1">
         <v>2130389</v>
       </c>
       <c r="H87" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3293,13 +3326,13 @@
         <v>15</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G88" s="1">
         <v>2130389</v>
       </c>
       <c r="H88" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3319,13 +3352,13 @@
         <v>15</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G89" s="1">
         <v>2130389</v>
       </c>
       <c r="H89" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3345,13 +3378,13 @@
         <v>15</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G90" s="1">
         <v>2130389</v>
       </c>
       <c r="H90" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3371,13 +3404,13 @@
         <v>15</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G91" s="1">
         <v>2130389</v>
       </c>
       <c r="H91" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3397,13 +3430,13 @@
         <v>15</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G92" s="1">
         <v>2130389</v>
       </c>
       <c r="H92" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3423,13 +3456,13 @@
         <v>15</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G93" s="1">
         <v>2130389</v>
       </c>
       <c r="H93" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3449,13 +3482,13 @@
         <v>15</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G94" s="1">
         <v>2130389</v>
       </c>
       <c r="H94" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3475,13 +3508,13 @@
         <v>15</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G95" s="1">
         <v>2130389</v>
       </c>
       <c r="H95" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3501,13 +3534,13 @@
         <v>15</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G96" s="1">
         <v>2130389</v>
       </c>
       <c r="H96" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3527,13 +3560,13 @@
         <v>15</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G97" s="1">
         <v>2130389</v>
       </c>
       <c r="H97" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3553,13 +3586,13 @@
         <v>15</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G98" s="1">
         <v>2130389</v>
       </c>
       <c r="H98" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3579,13 +3612,13 @@
         <v>15</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G99" s="1">
         <v>2130389</v>
       </c>
       <c r="H99" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3605,13 +3638,13 @@
         <v>15</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G100" s="1">
         <v>2130389</v>
       </c>
       <c r="H100" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3631,13 +3664,13 @@
         <v>15</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G101" s="1">
         <v>2130329</v>
       </c>
       <c r="H101" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3657,13 +3690,13 @@
         <v>15</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G102" s="1">
         <v>2130329</v>
       </c>
       <c r="H102" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3683,13 +3716,13 @@
         <v>15</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G103" s="1">
         <v>2130329</v>
       </c>
       <c r="H103" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3709,13 +3742,13 @@
         <v>15</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G104" s="1">
         <v>2130329</v>
       </c>
       <c r="H104" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3735,13 +3768,13 @@
         <v>15</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G105" s="1">
         <v>2130329</v>
       </c>
       <c r="H105" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3761,13 +3794,13 @@
         <v>15</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G106" s="1">
         <v>2130329</v>
       </c>
       <c r="H106" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3787,13 +3820,13 @@
         <v>15</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G107" s="1">
         <v>2130329</v>
       </c>
       <c r="H107" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3813,13 +3846,13 @@
         <v>15</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G108" s="1">
         <v>2130329</v>
       </c>
       <c r="H108" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3839,13 +3872,13 @@
         <v>15</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G109" s="1">
         <v>2130329</v>
       </c>
       <c r="H109" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3865,13 +3898,13 @@
         <v>15</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G110" s="1">
         <v>2130329</v>
       </c>
       <c r="H110" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3891,13 +3924,13 @@
         <v>15</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G111" s="1">
         <v>2130329</v>
       </c>
       <c r="H111" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3917,13 +3950,13 @@
         <v>15</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G112" s="1">
         <v>2130329</v>
       </c>
       <c r="H112" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3943,13 +3976,13 @@
         <v>15</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G113" s="1">
         <v>2130329</v>
       </c>
       <c r="H113" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3969,13 +4002,13 @@
         <v>15</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G114" s="1">
         <v>2130329</v>
       </c>
       <c r="H114" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -3995,13 +4028,13 @@
         <v>15</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G115" s="1">
         <v>2130329</v>
       </c>
       <c r="H115" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4021,13 +4054,13 @@
         <v>15</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G116" s="1">
         <v>2130329</v>
       </c>
       <c r="H116" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4047,13 +4080,13 @@
         <v>15</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G117" s="1">
         <v>2130329</v>
       </c>
       <c r="H117" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4073,13 +4106,13 @@
         <v>15</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G118" s="1">
         <v>2130329</v>
       </c>
       <c r="H118" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4099,13 +4132,13 @@
         <v>15</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G119" s="1">
         <v>2130329</v>
       </c>
       <c r="H119" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4125,13 +4158,13 @@
         <v>15</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G120" s="1">
         <v>2130329</v>
       </c>
       <c r="H120" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4151,13 +4184,13 @@
         <v>15</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G121" s="1">
         <v>2130329</v>
       </c>
       <c r="H121" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4177,13 +4210,13 @@
         <v>15</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G122" s="1">
         <v>2130329</v>
       </c>
       <c r="H122" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4203,13 +4236,13 @@
         <v>15</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G123" s="1">
         <v>2130329</v>
       </c>
       <c r="H123" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4229,13 +4262,13 @@
         <v>15</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G124" s="1">
         <v>2130329</v>
       </c>
       <c r="H124" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4255,13 +4288,13 @@
         <v>15</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G125" s="1">
         <v>2130329</v>
       </c>
       <c r="H125" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4281,13 +4314,13 @@
         <v>15</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G126" s="1">
         <v>2130329</v>
       </c>
       <c r="H126" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4307,13 +4340,13 @@
         <v>15</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G127" s="1">
         <v>2130329</v>
       </c>
       <c r="H127" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4333,13 +4366,13 @@
         <v>15</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G128" s="1">
         <v>2130329</v>
       </c>
       <c r="H128" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4359,13 +4392,13 @@
         <v>15</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G129" s="1">
         <v>2130329</v>
       </c>
       <c r="H129" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4385,13 +4418,13 @@
         <v>15</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G130" s="1">
         <v>2130329</v>
       </c>
       <c r="H130" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4411,13 +4444,13 @@
         <v>15</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G131" s="1">
         <v>2130329</v>
       </c>
       <c r="H131" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4437,13 +4470,13 @@
         <v>15</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G132" s="1">
         <v>2130329</v>
       </c>
       <c r="H132" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4463,13 +4496,13 @@
         <v>15</v>
       </c>
       <c r="F133" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G133" s="1">
         <v>1358043</v>
       </c>
       <c r="H133" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4489,13 +4522,13 @@
         <v>15</v>
       </c>
       <c r="F134" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G134" s="1">
         <v>1358043</v>
       </c>
       <c r="H134" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4515,13 +4548,13 @@
         <v>15</v>
       </c>
       <c r="F135" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G135" s="1">
         <v>1358043</v>
       </c>
       <c r="H135" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4541,13 +4574,13 @@
         <v>15</v>
       </c>
       <c r="F136" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G136" s="1">
         <v>1358043</v>
       </c>
       <c r="H136" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4567,13 +4600,13 @@
         <v>15</v>
       </c>
       <c r="F137" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G137" s="1">
         <v>1358043</v>
       </c>
       <c r="H137" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4593,13 +4626,13 @@
         <v>15</v>
       </c>
       <c r="F138" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G138" s="1">
         <v>1358043</v>
       </c>
       <c r="H138" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4619,13 +4652,13 @@
         <v>15</v>
       </c>
       <c r="F139" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G139" s="1">
         <v>1358043</v>
       </c>
       <c r="H139" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4645,13 +4678,13 @@
         <v>15</v>
       </c>
       <c r="F140" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G140" s="1">
         <v>1358043</v>
       </c>
       <c r="H140" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4671,13 +4704,13 @@
         <v>15</v>
       </c>
       <c r="F141" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G141" s="1">
         <v>1358043</v>
       </c>
       <c r="H141" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4697,13 +4730,13 @@
         <v>15</v>
       </c>
       <c r="F142" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G142" s="1">
         <v>1358043</v>
       </c>
       <c r="H142" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4723,13 +4756,13 @@
         <v>15</v>
       </c>
       <c r="F143" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G143" s="1">
         <v>1358043</v>
       </c>
       <c r="H143" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="144" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4749,13 +4782,13 @@
         <v>15</v>
       </c>
       <c r="F144" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G144" s="1">
         <v>1358043</v>
       </c>
       <c r="H144" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="145" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4775,13 +4808,13 @@
         <v>15</v>
       </c>
       <c r="F145" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G145" s="1">
         <v>1358043</v>
       </c>
       <c r="H145" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4801,13 +4834,13 @@
         <v>15</v>
       </c>
       <c r="F146" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G146" s="1">
         <v>1358043</v>
       </c>
       <c r="H146" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="147" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4827,13 +4860,13 @@
         <v>15</v>
       </c>
       <c r="F147" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G147" s="1">
         <v>1358043</v>
       </c>
       <c r="H147" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4853,13 +4886,13 @@
         <v>15</v>
       </c>
       <c r="F148" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G148" s="1">
         <v>1358043</v>
       </c>
       <c r="H148" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="149" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4879,13 +4912,13 @@
         <v>15</v>
       </c>
       <c r="F149" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G149" s="1">
         <v>1358043</v>
       </c>
       <c r="H149" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4905,13 +4938,13 @@
         <v>15</v>
       </c>
       <c r="F150" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G150" s="1">
         <v>1358043</v>
       </c>
       <c r="H150" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="151" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4931,13 +4964,13 @@
         <v>15</v>
       </c>
       <c r="F151" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G151" s="1">
         <v>1358043</v>
       </c>
       <c r="H151" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="152" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4957,13 +4990,13 @@
         <v>15</v>
       </c>
       <c r="F152" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G152" s="1">
         <v>1358043</v>
       </c>
       <c r="H152" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -4983,13 +5016,13 @@
         <v>15</v>
       </c>
       <c r="F153" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G153" s="1">
         <v>1358043</v>
       </c>
       <c r="H153" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5009,13 +5042,13 @@
         <v>15</v>
       </c>
       <c r="F154" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G154" s="1">
         <v>1358043</v>
       </c>
       <c r="H154" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="155" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5035,13 +5068,13 @@
         <v>15</v>
       </c>
       <c r="F155" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G155" s="1">
         <v>1358043</v>
       </c>
       <c r="H155" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="156" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5061,13 +5094,13 @@
         <v>15</v>
       </c>
       <c r="F156" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G156" s="1">
         <v>1358043</v>
       </c>
       <c r="H156" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="157" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5087,13 +5120,13 @@
         <v>15</v>
       </c>
       <c r="F157" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G157" s="1">
         <v>1358043</v>
       </c>
       <c r="H157" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="158" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5113,13 +5146,13 @@
         <v>15</v>
       </c>
       <c r="F158" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G158" s="1">
         <v>1358043</v>
       </c>
       <c r="H158" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="159" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5139,13 +5172,13 @@
         <v>15</v>
       </c>
       <c r="F159" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G159" s="1">
         <v>1358043</v>
       </c>
       <c r="H159" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="160" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5165,13 +5198,13 @@
         <v>15</v>
       </c>
       <c r="F160" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G160" s="1">
         <v>1358043</v>
       </c>
       <c r="H160" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="161" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5191,13 +5224,13 @@
         <v>15</v>
       </c>
       <c r="F161" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G161" s="1">
         <v>1358043</v>
       </c>
       <c r="H161" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="162" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5217,13 +5250,13 @@
         <v>15</v>
       </c>
       <c r="F162" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G162" s="1">
         <v>1358043</v>
       </c>
       <c r="H162" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="163" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5243,13 +5276,13 @@
         <v>15</v>
       </c>
       <c r="F163" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G163" s="1">
         <v>1358043</v>
       </c>
       <c r="H163" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="164" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5269,13 +5302,13 @@
         <v>15</v>
       </c>
       <c r="F164" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G164" s="1">
         <v>1358043</v>
       </c>
       <c r="H164" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="165" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -5283,7 +5316,7 @@
         <v>176</v>
       </c>
       <c r="B165" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="C165" t="s">
         <v>13</v>
@@ -5294,22 +5327,20 @@
       <c r="E165" t="s">
         <v>15</v>
       </c>
-      <c r="F165" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G165" s="1">
-        <v>2130550</v>
-      </c>
+      <c r="F165" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="G165" s="1"/>
       <c r="H165" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="166" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B166" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="C166" t="s">
         <v>13</v>
@@ -5320,22 +5351,20 @@
       <c r="E166" t="s">
         <v>15</v>
       </c>
-      <c r="F166" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G166" s="1">
-        <v>2130550</v>
-      </c>
+      <c r="F166" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="G166" s="1"/>
       <c r="H166" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="167" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B167" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="C167" t="s">
         <v>13</v>
@@ -5346,22 +5375,20 @@
       <c r="E167" t="s">
         <v>15</v>
       </c>
-      <c r="F167" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G167" s="1">
-        <v>2130550</v>
-      </c>
+      <c r="F167" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="G167" s="1"/>
       <c r="H167" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="168" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B168" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C168" t="s">
         <v>13</v>
@@ -5372,19 +5399,17 @@
       <c r="E168" t="s">
         <v>15</v>
       </c>
-      <c r="F168" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="G168" s="1">
-        <v>2350493</v>
-      </c>
+      <c r="F168" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="G168" s="1"/>
       <c r="H168" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="169" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B169" t="s">
         <v>199</v>
@@ -5398,22 +5423,20 @@
       <c r="E169" t="s">
         <v>15</v>
       </c>
-      <c r="F169" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G169" s="1">
-        <v>2130463</v>
-      </c>
+      <c r="F169" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="G169" s="1"/>
       <c r="H169" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="170" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B170" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="C170" t="s">
         <v>13</v>
@@ -5424,22 +5447,20 @@
       <c r="E170" t="s">
         <v>15</v>
       </c>
-      <c r="F170" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G170" s="1">
-        <v>2350332</v>
-      </c>
+      <c r="F170" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="G170" s="1"/>
       <c r="H170" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B171" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="C171" t="s">
         <v>13</v>
@@ -5450,22 +5471,20 @@
       <c r="E171" t="s">
         <v>15</v>
       </c>
-      <c r="F171" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G171" s="1">
-        <v>2350332</v>
-      </c>
+      <c r="F171" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="G171" s="1"/>
       <c r="H171" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="172" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>186</v>
-      </c>
-      <c r="B172" t="s">
-        <v>184</v>
+        <v>183</v>
+      </c>
+      <c r="B172">
+        <v>500</v>
       </c>
       <c r="C172" t="s">
         <v>13</v>
@@ -5476,22 +5495,20 @@
       <c r="E172" t="s">
         <v>15</v>
       </c>
-      <c r="F172" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G172" s="1">
-        <v>2350332</v>
-      </c>
+      <c r="F172" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G172" s="1"/>
       <c r="H172" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="173" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>187</v>
-      </c>
-      <c r="B173" t="s">
-        <v>182</v>
+        <v>184</v>
+      </c>
+      <c r="B173">
+        <v>500</v>
       </c>
       <c r="C173" t="s">
         <v>13</v>
@@ -5502,22 +5519,20 @@
       <c r="E173" t="s">
         <v>15</v>
       </c>
-      <c r="F173" s="2" t="s">
+      <c r="F173" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="G173" s="1">
-        <v>2130431</v>
-      </c>
+      <c r="G173" s="1"/>
       <c r="H173" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="174" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>188</v>
-      </c>
-      <c r="B174" t="s">
-        <v>80</v>
+        <v>185</v>
+      </c>
+      <c r="B174">
+        <v>100</v>
       </c>
       <c r="C174" t="s">
         <v>13</v>
@@ -5528,22 +5543,20 @@
       <c r="E174" t="s">
         <v>15</v>
       </c>
-      <c r="F174" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G174" s="1">
-        <v>2130389</v>
-      </c>
+      <c r="F174" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G174" s="1"/>
       <c r="H174" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="175" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>189</v>
-      </c>
-      <c r="B175" t="s">
-        <v>80</v>
+        <v>186</v>
+      </c>
+      <c r="B175">
+        <v>100</v>
       </c>
       <c r="C175" t="s">
         <v>13</v>
@@ -5554,22 +5567,20 @@
       <c r="E175" t="s">
         <v>15</v>
       </c>
-      <c r="F175" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G175" s="1">
-        <v>2130389</v>
-      </c>
+      <c r="F175" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G175" s="1"/>
       <c r="H175" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="176" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>190</v>
-      </c>
-      <c r="B176" t="s">
-        <v>80</v>
+        <v>187</v>
+      </c>
+      <c r="B176">
+        <v>200</v>
       </c>
       <c r="C176" t="s">
         <v>13</v>
@@ -5580,28 +5591,26 @@
       <c r="E176" t="s">
         <v>15</v>
       </c>
-      <c r="F176" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G176" s="1">
-        <v>2130389</v>
-      </c>
+      <c r="F176" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="G176" s="1"/>
       <c r="H176" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="180" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E180" t="s">
-        <v>205</v>
-      </c>
-      <c r="F180">
+        <v>195</v>
+      </c>
+      <c r="F180" t="e">
         <f t="array" ref="F180">SUM(1/COUNTIF(G2:G176,G2:G176))</f>
-        <v>8.9999999999999947</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="181" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E181" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="F181">
         <f t="array" ref="F181" xml:space="preserve"> COUNTIF(H2:H176,"PCB*")</f>
@@ -5610,7 +5619,7 @@
     </row>
     <row r="182" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E182" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="F182">
         <f t="array" ref="F182">COUNTBLANK(H2:H176)</f>
@@ -5619,11 +5628,11 @@
     </row>
     <row r="183" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E183" t="s">
-        <v>208</v>
-      </c>
-      <c r="F183">
+        <v>198</v>
+      </c>
+      <c r="F183" t="e">
         <f t="array" ref="F183">SUM(F180:F182)</f>
-        <v>184</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>